<commit_message>
http2 a, b both
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -544,10 +544,10 @@
         <v>0.007806471605960011</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.0771084578037262</v>
+        <v>0.07475761151313781</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0.0147235377306453</v>
+        <v>0.02206291961922436</v>
       </c>
     </row>
     <row r="5">
@@ -563,10 +563,10 @@
         <v>0.008904034606921674</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>0.07339831113815308</v>
+        <v>0.08424967050552368</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.0143129866678803</v>
+        <v>0.01959415137762406</v>
       </c>
     </row>
     <row r="6">
@@ -582,10 +582,10 @@
         <v>0.01291177970381826</v>
       </c>
       <c r="D6" t="n">
-        <v>0.07742350101470948</v>
+        <v>0.09851876497268677</v>
       </c>
       <c r="E6" t="n">
-        <v>0.003779855344270848</v>
+        <v>0.03453666244963857</v>
       </c>
     </row>
     <row r="7">
@@ -601,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1836450099945068</v>
+        <v>0.3237078189849854</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -695,10 +695,10 @@
         <v>646260.6054127052</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>136602.3459554465</v>
+        <v>143886.396252974</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>21623.04111710057</v>
+        <v>25727.35812289039</v>
       </c>
     </row>
     <row r="5">
@@ -714,10 +714,10 @@
         <v>4537136.224672033</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>1439566.853030773</v>
+        <v>1288859.973798563</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>250589.5364854026</v>
+        <v>250854.3482564982</v>
       </c>
     </row>
     <row r="6">
@@ -733,10 +733,10 @@
         <v>10578558.70182016</v>
       </c>
       <c r="D6" t="n">
-        <v>13572472.95098387</v>
+        <v>11844353.21478873</v>
       </c>
       <c r="E6" t="n">
-        <v>663004.9964235323</v>
+        <v>2833977.45282994</v>
       </c>
     </row>
     <row r="7">
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>57097984.85847042</v>
+        <v>36648994.14349551</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
remove all json for http2
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -544,10 +544,10 @@
         <v>0.007806471605960011</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.07475761151313781</v>
+        <v>0.05301385378837584</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0.02206291961922436</v>
+        <v>0.0181948601778117</v>
       </c>
     </row>
     <row r="5">
@@ -563,10 +563,10 @@
         <v>0.008904034606921674</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>0.08424967050552368</v>
+        <v>0.06008161147435506</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.01959415137762406</v>
+        <v>0.01625077162169275</v>
       </c>
     </row>
     <row r="6">
@@ -582,10 +582,10 @@
         <v>0.01291177970381826</v>
       </c>
       <c r="D6" t="n">
-        <v>0.09851876497268677</v>
+        <v>0.07484465440114339</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03453666244963857</v>
+        <v>0.02859260297602438</v>
       </c>
     </row>
     <row r="7">
@@ -601,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3237078189849854</v>
+        <v>0.2778883775075277</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -695,10 +695,10 @@
         <v>646260.6054127052</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>143886.396252974</v>
+        <v>520624.680452256</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>25727.35812289039</v>
+        <v>284716.0199583442</v>
       </c>
     </row>
     <row r="5">
@@ -714,10 +714,10 @@
         <v>4537136.224672033</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>1288859.973798563</v>
+        <v>4283026.65530466</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>250854.3482564982</v>
+        <v>2377911.572522989</v>
       </c>
     </row>
     <row r="6">
@@ -733,10 +733,10 @@
         <v>10578558.70182016</v>
       </c>
       <c r="D6" t="n">
-        <v>11844353.21478873</v>
+        <v>21604097.78833389</v>
       </c>
       <c r="E6" t="n">
-        <v>2833977.45282994</v>
+        <v>7079283.594072331</v>
       </c>
     </row>
     <row r="7">
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>36648994.14349551</v>
+        <v>43199174.54121726</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
new result with http2
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -544,10 +544,10 @@
         <v>0.007806471605960011</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.05301385378837584</v>
+        <v>0.008527708172798156</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0.0181948601778117</v>
+        <v>0.003864228111583123</v>
       </c>
     </row>
     <row r="5">
@@ -563,10 +563,10 @@
         <v>0.008904034606921674</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>0.06008161147435506</v>
+        <v>0.01721251964569092</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.01625077162169275</v>
+        <v>0.01080990045973373</v>
       </c>
     </row>
     <row r="6">
@@ -582,10 +582,10 @@
         <v>0.01291177970381826</v>
       </c>
       <c r="D6" t="n">
-        <v>0.07484465440114339</v>
+        <v>0.1141218423843384</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02859260297602438</v>
+        <v>0.02248933364168916</v>
       </c>
     </row>
     <row r="7">
@@ -601,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2778883775075277</v>
+        <v>0.9106026887893677</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -695,10 +695,10 @@
         <v>646260.6054127052</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>520624.680452256</v>
+        <v>1406182.728407707</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>284716.0199583442</v>
+        <v>515828.0395166186</v>
       </c>
     </row>
     <row r="5">
@@ -714,10 +714,10 @@
         <v>4537136.224672033</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>4283026.65530466</v>
+        <v>6991508.194169387</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>2377911.572522989</v>
+        <v>2265222.321775638</v>
       </c>
     </row>
     <row r="6">
@@ -733,10 +733,10 @@
         <v>10578558.70182016</v>
       </c>
       <c r="D6" t="n">
-        <v>21604097.78833389</v>
+        <v>9829286.040962379</v>
       </c>
       <c r="E6" t="n">
-        <v>7079283.594072331</v>
+        <v>1864039.675413585</v>
       </c>
     </row>
     <row r="7">
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>43199174.54121726</v>
+        <v>11568075.78619621</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -846,10 +846,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>1.02626953125</v>
+        <v>1.020264990234375</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0</v>
+        <v>4.171876828768403e-05</v>
       </c>
     </row>
     <row r="5">
@@ -865,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>1.00263671875</v>
+        <v>1.0025732421875</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.000258445739746</v>
+        <v>1.000741004943848</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.000025939941406</v>
+        <v>1.000568580627441</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
ssl results added too
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,8 @@
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -500,6 +502,12 @@
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>HTTP/2 SSL</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -519,6 +527,16 @@
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Std Dev</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Std Dev</t>
         </is>
@@ -530,6 +548,8 @@
       <c r="C3" s="3" t="n"/>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -549,6 +569,12 @@
       <c r="E4" s="4" t="n">
         <v>0.003864228111583123</v>
       </c>
+      <c r="F4" s="4" t="n">
+        <v>0.01700205326080322</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0.01556676824206549</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -568,6 +594,12 @@
       <c r="E5" s="4" t="n">
         <v>0.01080990045973373</v>
       </c>
+      <c r="F5" s="4" t="n">
+        <v>0.02456668138504028</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>0.01307115455139281</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
@@ -587,6 +619,12 @@
       <c r="E6" t="n">
         <v>0.02248933364168916</v>
       </c>
+      <c r="F6" t="n">
+        <v>0.1406377077102661</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.04032567721202485</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
@@ -606,10 +644,17 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
+      <c r="F7" t="n">
+        <v>1.726834058761597</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -622,7 +667,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -635,6 +680,8 @@
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -651,6 +698,12 @@
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>HTTP/2 SSL</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -670,6 +723,16 @@
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Std Dev</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Std Dev</t>
         </is>
@@ -681,6 +744,8 @@
       <c r="C3" s="3" t="n"/>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -700,6 +765,12 @@
       <c r="E4" s="6" t="n">
         <v>515828.0395166186</v>
       </c>
+      <c r="F4" s="6" t="n">
+        <v>857495.5432740636</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>377229.6488290807</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -719,6 +790,12 @@
       <c r="E5" s="6" t="n">
         <v>2265222.321775638</v>
       </c>
+      <c r="F5" s="6" t="n">
+        <v>4819337.391183397</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>1522637.096039632</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
@@ -738,6 +815,12 @@
       <c r="E6" t="n">
         <v>1864039.675413585</v>
       </c>
+      <c r="F6" t="n">
+        <v>7967923.367428995</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1978908.963937275</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
@@ -757,10 +840,17 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
+      <c r="F7" t="n">
+        <v>7469176.729335703</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -773,7 +863,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -786,6 +876,8 @@
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -802,6 +894,12 @@
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>HTTP/2 SSL</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -821,6 +919,16 @@
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Std Dev</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Std Dev</t>
         </is>
@@ -832,6 +940,8 @@
       <c r="C3" s="3" t="n"/>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -851,6 +961,12 @@
       <c r="E4" s="4" t="n">
         <v>4.171876828768403e-05</v>
       </c>
+      <c r="F4" s="4" t="n">
+        <v>1.0212890625</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -870,6 +986,12 @@
       <c r="E5" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F5" s="4" t="n">
+        <v>1.00267578125</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
@@ -889,6 +1011,12 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
+      <c r="F6" t="n">
+        <v>1.000751495361328</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
@@ -908,10 +1036,17 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
+      <c r="F7" t="n">
+        <v>1.000569629669189</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated with http2 non ssl
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -498,13 +498,13 @@
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/2</t>
+          <t>HTTP/2 SSL</t>
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/2 SSL</t>
+          <t>HTTP/2</t>
         </is>
       </c>
       <c r="G1" s="1" t="n"/>
@@ -564,16 +564,16 @@
         <v>0.007806471605960011</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.008527708172798156</v>
+        <v>0.01860912831624349</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0.003864228111583123</v>
+        <v>0.01781765832560506</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>0.01700205326080322</v>
+        <v>0.0108374330997467</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>0.01556676824206549</v>
+        <v>0.00646512990140088</v>
       </c>
     </row>
     <row r="5">
@@ -589,16 +589,16 @@
         <v>0.008904034606921674</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>0.01721251964569092</v>
+        <v>0.02502824942270915</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.01080990045973373</v>
+        <v>0.01429187471737145</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>0.02456668138504028</v>
+        <v>0.01645312070846558</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>0.01307115455139281</v>
+        <v>0.006651154588850086</v>
       </c>
     </row>
     <row r="6">
@@ -614,16 +614,16 @@
         <v>0.01291177970381826</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1141218423843384</v>
+        <v>0.1433880964914958</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02248933364168916</v>
+        <v>0.04356813924271643</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1406377077102661</v>
+        <v>0.09403650760650635</v>
       </c>
       <c r="G6" t="n">
-        <v>0.04032567721202485</v>
+        <v>0.005134282398925803</v>
       </c>
     </row>
     <row r="7">
@@ -639,13 +639,13 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9106026887893677</v>
+        <v>1.975765943527222</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1.726834058761597</v>
+        <v>0.7036097049713135</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -694,13 +694,13 @@
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/2</t>
+          <t>HTTP/2 SSL</t>
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/2 SSL</t>
+          <t>HTTP/2</t>
         </is>
       </c>
       <c r="G1" s="1" t="n"/>
@@ -760,16 +760,16 @@
         <v>646260.6054127052</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>1406182.728407707</v>
+        <v>829991.1173650185</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>515828.0395166186</v>
+        <v>394289.2181876033</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>857495.5432740636</v>
+        <v>1187626.088236784</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>377229.6488290807</v>
+        <v>529051.1059366131</v>
       </c>
     </row>
     <row r="5">
@@ -785,16 +785,16 @@
         <v>4537136.224672033</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>6991508.194169387</v>
+        <v>4802910.522485345</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>2265222.321775638</v>
+        <v>1558273.501772276</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>4819337.391183397</v>
+        <v>6910514.160241783</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>1522637.096039632</v>
+        <v>2019480.877227425</v>
       </c>
     </row>
     <row r="6">
@@ -810,16 +810,16 @@
         <v>10578558.70182016</v>
       </c>
       <c r="D6" t="n">
-        <v>9829286.040962379</v>
+        <v>7891914.411074576</v>
       </c>
       <c r="E6" t="n">
-        <v>1864039.675413585</v>
+        <v>2129848.297298706</v>
       </c>
       <c r="F6" t="n">
-        <v>7967923.367428995</v>
+        <v>11181189.72082671</v>
       </c>
       <c r="G6" t="n">
-        <v>1978908.963937275</v>
+        <v>622199.0804710645</v>
       </c>
     </row>
     <row r="7">
@@ -835,13 +835,13 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>11568075.78619621</v>
+        <v>6392457.03444244</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>7469176.729335703</v>
+        <v>14902807.51660114</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -890,13 +890,13 @@
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/2</t>
+          <t>HTTP/2 SSL</t>
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/2 SSL</t>
+          <t>HTTP/2</t>
         </is>
       </c>
       <c r="G1" s="1" t="n"/>
@@ -956,16 +956,16 @@
         <v>0</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>1.020264990234375</v>
+        <v>1.021321614583333</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>4.171876828768403e-05</v>
+        <v>0</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>1.0212890625</v>
+        <v>1.02021611328125</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>0</v>
+        <v>4.014610310760497e-05</v>
       </c>
     </row>
     <row r="5">
@@ -981,13 +981,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>1.0025732421875</v>
+        <v>1.00267578125</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>1.00267578125</v>
+        <v>1.002568359375</v>
       </c>
       <c r="G5" s="4" t="n">
         <v>0</v>
@@ -1006,13 +1006,13 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
+        <v>1.000751495361328</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
         <v>1.000741004943848</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1.000751495361328</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1031,13 +1031,13 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
+        <v>1.000569629669189</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
         <v>1.000568580627441</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1.000569629669189</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
new results with http1.1 and http2
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,8 +484,6 @@
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -498,16 +496,10 @@
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/2 SSL</t>
+          <t>HTTP/2</t>
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>HTTP/2</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -527,16 +519,6 @@
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>Std Dev</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>Mean</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Std Dev</t>
         </is>
@@ -548,8 +530,6 @@
       <c r="C3" s="3" t="n"/>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -558,22 +538,16 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>0.01010183238983154</v>
+        <v>0.01056118428707123</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>0.007806471605960011</v>
+        <v>0.005242367281925539</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.01860912831624349</v>
+        <v>0.01389548802375793</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0.01781765832560506</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>0.0108374330997467</v>
-      </c>
-      <c r="G4" s="4" t="n">
-        <v>0.00646512990140088</v>
+        <v>0.01750155598801064</v>
       </c>
     </row>
     <row r="5">
@@ -583,22 +557,16 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>0.01291730523109436</v>
+        <v>0.01183918118476868</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>0.008904034606921674</v>
+        <v>0.006374975155080995</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>0.02502824942270915</v>
+        <v>0.04640535354614258</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.01429187471737145</v>
-      </c>
-      <c r="F5" s="4" t="n">
-        <v>0.01645312070846558</v>
-      </c>
-      <c r="G5" s="4" t="n">
-        <v>0.006651154588850086</v>
+        <v>0.01160893773458314</v>
       </c>
     </row>
     <row r="6">
@@ -608,22 +576,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.02944159507751465</v>
+        <v>0.03155416250228882</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01291177970381826</v>
+        <v>0.01692662311134954</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1433880964914958</v>
+        <v>0.09788004159927369</v>
       </c>
       <c r="E6" t="n">
-        <v>0.04356813924271643</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.09403650760650635</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.005134282398925803</v>
+        <v>0.01815001640077183</v>
       </c>
     </row>
     <row r="7">
@@ -633,28 +595,21 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1560657024383545</v>
+        <v>0.3036929368972778</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.975765943527222</v>
+        <v>3.874284625053406</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="n">
-        <v>0.7036097049713135</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -667,7 +622,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -680,8 +635,6 @@
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -694,16 +647,10 @@
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/2 SSL</t>
+          <t>HTTP/2</t>
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>HTTP/2</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -723,16 +670,6 @@
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>Std Dev</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>Mean</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Std Dev</t>
         </is>
@@ -744,8 +681,6 @@
       <c r="C3" s="3" t="n"/>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -754,22 +689,16 @@
         </is>
       </c>
       <c r="B4" s="6" t="n">
-        <v>1397958.397601407</v>
+        <v>9255521.730111934</v>
       </c>
       <c r="C4" s="6" t="n">
-        <v>646260.6054127052</v>
+        <v>3680421.788750582</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>829991.1173650185</v>
+        <v>20744932.44065881</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>394289.2181876033</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>1187626.088236784</v>
-      </c>
-      <c r="G4" s="6" t="n">
-        <v>529051.1059366131</v>
+        <v>14488310.68536471</v>
       </c>
     </row>
     <row r="5">
@@ -779,22 +708,16 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>11328528.42127636</v>
+        <v>84427327.22572178</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>4537136.224672033</v>
+        <v>33649506.05929364</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>4802910.522485345</v>
+        <v>23825560.63408853</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>1558273.501772276</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>6910514.160241783</v>
-      </c>
-      <c r="G5" s="6" t="n">
-        <v>2019480.877227425</v>
+        <v>28432632.23320282</v>
       </c>
     </row>
     <row r="6">
@@ -804,22 +727,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>40242737.21188971</v>
+        <v>308957763.0495739</v>
       </c>
       <c r="C6" t="n">
-        <v>10578558.70182016</v>
+        <v>95561058.99782108</v>
       </c>
       <c r="D6" t="n">
-        <v>7891914.411074576</v>
+        <v>88122599.94104275</v>
       </c>
       <c r="E6" t="n">
-        <v>2129848.297298706</v>
-      </c>
-      <c r="F6" t="n">
-        <v>11181189.72082671</v>
-      </c>
-      <c r="G6" t="n">
-        <v>622199.0804710645</v>
+        <v>13777981.31061908</v>
       </c>
     </row>
     <row r="7">
@@ -829,28 +746,21 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>70382965.18229568</v>
+        <v>276513431.7404806</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>6392457.03444244</v>
+        <v>21962448.46551479</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="n">
-        <v>14902807.51660114</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -863,7 +773,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -876,8 +786,6 @@
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -890,16 +798,10 @@
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/2 SSL</t>
+          <t>HTTP/2</t>
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>HTTP/2</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -919,16 +821,6 @@
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>Std Dev</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>Mean</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Std Dev</t>
         </is>
@@ -940,8 +832,6 @@
       <c r="C3" s="3" t="n"/>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -956,16 +846,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>1.021321614583333</v>
+        <v>1.00908203125</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>0</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>1.02021611328125</v>
-      </c>
-      <c r="G4" s="4" t="n">
-        <v>4.014610310760497e-05</v>
       </c>
     </row>
     <row r="5">
@@ -981,15 +865,9 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>1.00267578125</v>
+        <v>1.00091796875</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4" t="n">
-        <v>1.002568359375</v>
-      </c>
-      <c r="G5" s="4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1006,15 +884,9 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.000751495361328</v>
+        <v>1.000090599060059</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1.000741004943848</v>
-      </c>
-      <c r="G6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1031,22 +903,15 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.000569629669189</v>
+        <v>1.000009155273438</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="n">
-        <v>1.000568580627441</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated the all http result
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>0.01056118428707123</v>
+        <v>0.009963054299354554</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>0.005242367281925539</v>
+        <v>0.005181819649484069</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.01389548802375793</v>
+        <v>0.01418705487251282</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0.01750155598801064</v>
+        <v>0.01797109972563448</v>
       </c>
     </row>
     <row r="5">
@@ -557,16 +557,16 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>0.01183918118476868</v>
+        <v>0.01323233366012573</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>0.006374975155080995</v>
+        <v>0.005749628294880777</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>0.04640535354614258</v>
+        <v>0.04627740144729614</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.01160893773458314</v>
+        <v>0.01178264574478354</v>
       </c>
     </row>
     <row r="6">
@@ -576,16 +576,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.03155416250228882</v>
+        <v>0.02930171489715576</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01692662311134954</v>
+        <v>0.01060076133917406</v>
       </c>
       <c r="D6" t="n">
-        <v>0.09788004159927369</v>
+        <v>0.1010946869850159</v>
       </c>
       <c r="E6" t="n">
-        <v>0.01815001640077183</v>
+        <v>0.02983875185514805</v>
       </c>
     </row>
     <row r="7">
@@ -595,13 +595,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3036929368972778</v>
+        <v>0.1984585523605347</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>3.874284625053406</v>
+        <v>2.159919381141663</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -689,16 +689,16 @@
         </is>
       </c>
       <c r="B4" s="6" t="n">
-        <v>9255521.730111934</v>
+        <v>9827463.639666218</v>
       </c>
       <c r="C4" s="6" t="n">
-        <v>3680421.788750582</v>
+        <v>3817495.177306633</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>20744932.44065881</v>
+        <v>20321686.671219</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>14488310.68536471</v>
+        <v>14653429.31618624</v>
       </c>
     </row>
     <row r="5">
@@ -708,16 +708,16 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>84427327.22572178</v>
+        <v>73611763.66876601</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>33649506.05929364</v>
+        <v>30069905.29991582</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>23825560.63408853</v>
+        <v>22454243.5859525</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>28432632.23320282</v>
+        <v>21727084.20517864</v>
       </c>
     </row>
     <row r="6">
@@ -727,16 +727,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>308957763.0495739</v>
+        <v>324711003.9069602</v>
       </c>
       <c r="C6" t="n">
-        <v>95561058.99782108</v>
+        <v>114405569.2885726</v>
       </c>
       <c r="D6" t="n">
-        <v>88122599.94104275</v>
+        <v>86919085.30927305</v>
       </c>
       <c r="E6" t="n">
-        <v>13777981.31061908</v>
+        <v>15208536.58317422</v>
       </c>
     </row>
     <row r="7">
@@ -746,13 +746,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>276513431.7404806</v>
+        <v>425548546.5109209</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>21962448.46551479</v>
+        <v>38837619.61538628</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>1.03974609375</v>
+        <v>1.0396484375</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>0</v>
@@ -859,7 +859,7 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>1.003994140625</v>
+        <v>1.003984375</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>0</v>
@@ -878,7 +878,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.000389099121094</v>
+        <v>1.000388145446777</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.000039100646973</v>
+        <v>1.000039005279541</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Update results.xlsx with new data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,13 +484,15 @@
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/1.1</t>
+          <t>p2p BitTorrent</t>
         </is>
       </c>
       <c r="C1" s="1" t="n"/>
@@ -500,6 +502,12 @@
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>HTTP/1.1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -519,6 +527,16 @@
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Std Dev</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Std Dev</t>
         </is>
@@ -530,6 +548,8 @@
       <c r="C3" s="3" t="n"/>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -537,18 +557,20 @@
           <t>10kB</t>
         </is>
       </c>
-      <c r="B4" s="4" t="n">
-        <v>0.009963054299354554</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>0.005181819649484069</v>
-      </c>
+      <c r="B4" s="3" t="inlineStr"/>
+      <c r="C4" s="3" t="inlineStr"/>
       <c r="D4" s="4" t="n">
         <v>0.01418705487251282</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>0.01797109972563448</v>
       </c>
+      <c r="F4" s="4" t="n">
+        <v>0.009963054299354554</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0.005181819649484069</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -556,18 +578,20 @@
           <t>100kB</t>
         </is>
       </c>
-      <c r="B5" s="4" t="n">
-        <v>0.01323233366012573</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>0.005749628294880777</v>
-      </c>
+      <c r="B5" s="3" t="inlineStr"/>
+      <c r="C5" s="3" t="inlineStr"/>
       <c r="D5" s="4" t="n">
         <v>0.04627740144729614</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>0.01178264574478354</v>
       </c>
+      <c r="F5" s="4" t="n">
+        <v>0.01323233366012573</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>0.005749628294880777</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
@@ -576,10 +600,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.02930171489715576</v>
+        <v>2.349340756734212</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01060076133917406</v>
+        <v>0.6341095253989198</v>
       </c>
       <c r="D6" t="n">
         <v>0.1010946869850159</v>
@@ -587,6 +611,12 @@
       <c r="E6" t="n">
         <v>0.02983875185514805</v>
       </c>
+      <c r="F6" t="n">
+        <v>0.02930171489715576</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.01060076133917406</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
@@ -595,7 +625,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1984585523605347</v>
+        <v>4.431923389434814</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -606,10 +636,17 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
+      <c r="F7" t="n">
+        <v>0.1984585523605347</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -622,7 +659,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -635,13 +672,15 @@
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/1.1</t>
+          <t>p2p BitTorrent</t>
         </is>
       </c>
       <c r="C1" s="1" t="n"/>
@@ -651,6 +690,12 @@
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>HTTP/1.1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -670,6 +715,16 @@
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Std Dev</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Std Dev</t>
         </is>
@@ -681,6 +736,8 @@
       <c r="C3" s="3" t="n"/>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -688,18 +745,20 @@
           <t>10kB</t>
         </is>
       </c>
-      <c r="B4" s="6" t="n">
-        <v>9827463.639666218</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>3817495.177306633</v>
-      </c>
+      <c r="B4" s="3" t="inlineStr"/>
+      <c r="C4" s="3" t="inlineStr"/>
       <c r="D4" s="6" t="n">
         <v>20321686.671219</v>
       </c>
       <c r="E4" s="6" t="n">
         <v>14653429.31618624</v>
       </c>
+      <c r="F4" s="6" t="n">
+        <v>9827463.639666218</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>3817495.177306633</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -707,18 +766,20 @@
           <t>100kB</t>
         </is>
       </c>
-      <c r="B5" s="6" t="n">
-        <v>73611763.66876601</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>30069905.29991582</v>
-      </c>
+      <c r="B5" s="3" t="inlineStr"/>
+      <c r="C5" s="3" t="inlineStr"/>
       <c r="D5" s="6" t="n">
         <v>22454243.5859525</v>
       </c>
       <c r="E5" s="6" t="n">
         <v>21727084.20517864</v>
       </c>
+      <c r="F5" s="6" t="n">
+        <v>73611763.66876601</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>30069905.29991582</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
@@ -727,10 +788,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>324711003.9069602</v>
+        <v>10114.69803173217</v>
       </c>
       <c r="C6" t="n">
-        <v>114405569.2885726</v>
+        <v>3435.038111728009</v>
       </c>
       <c r="D6" t="n">
         <v>86919085.30927305</v>
@@ -738,6 +799,12 @@
       <c r="E6" t="n">
         <v>15208536.58317422</v>
       </c>
+      <c r="F6" t="n">
+        <v>324711003.9069602</v>
+      </c>
+      <c r="G6" t="n">
+        <v>114405569.2885726</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
@@ -746,7 +813,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>425548546.5109209</v>
+        <v>56635.20281022038</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -757,10 +824,17 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
+      <c r="F7" t="n">
+        <v>425548546.5109209</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -773,7 +847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -786,13 +860,15 @@
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>HTTP/1.1</t>
+          <t>p2p BitTorrent</t>
         </is>
       </c>
       <c r="C1" s="1" t="n"/>
@@ -802,6 +878,12 @@
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>HTTP/1.1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -821,6 +903,16 @@
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Std Dev</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Std Dev</t>
         </is>
@@ -832,6 +924,8 @@
       <c r="C3" s="3" t="n"/>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -839,18 +933,20 @@
           <t>10kB</t>
         </is>
       </c>
-      <c r="B4" s="4" t="n">
-        <v>1.0396484375</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="B4" s="3" t="inlineStr"/>
+      <c r="C4" s="3" t="inlineStr"/>
       <c r="D4" s="4" t="n">
         <v>1.00908203125</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F4" s="4" t="n">
+        <v>1.0396484375</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -858,18 +954,20 @@
           <t>100kB</t>
         </is>
       </c>
-      <c r="B5" s="4" t="n">
-        <v>1.003984375</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="B5" s="3" t="inlineStr"/>
+      <c r="C5" s="3" t="inlineStr"/>
       <c r="D5" s="4" t="n">
         <v>1.00091796875</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F5" s="4" t="n">
+        <v>1.003984375</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
@@ -878,10 +976,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.000388145446777</v>
+        <v>1.00267129492618</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.00014128277808102</v>
       </c>
       <c r="D6" t="n">
         <v>1.000090599060059</v>
@@ -889,6 +987,12 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
+      <c r="F6" t="n">
+        <v>1.000388145446777</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
@@ -897,7 +1001,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.000039005279541</v>
+        <v>1.00177945368595</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -908,10 +1012,17 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
+      <c r="F7" t="n">
+        <v>1.000039005279541</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>